<commit_message>
agregar modo de bloqueo en la aplicación y actualizar el botón EX1 a LOCK
</commit_message>
<xml_diff>
--- a/REVs/REV-17-03-2025.xlsx
+++ b/REVs/REV-17-03-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,20 +784,569 @@
           <t>GR</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0ML34254</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0ML34251</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0ML34257</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 8</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0ML34253</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 3</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0ML34258</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0ML34252</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 2</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0ML34255</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 6</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0ML34256</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 7</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0ML34251</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0ML34257</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>YSL LOVESHINE PLUMPING GLOSS N 8</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TESTE-EAN</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE LABIOS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>TESTE Desc PT</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>TESTE Uso PT</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>TESTE prec PT</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>TESTE +info PT</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>TESTE desc IT</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>TESTE uso IT</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>TESTE preca IT</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>TESTE +info IT</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Aislado de V3 verison estable, script para migrar base de datos de SQLite a Excel sebtido reverso y agregar manejo de excepciones en la aplicación
</commit_message>
<xml_diff>
--- a/REVs/REV-17-03-2025.xlsx
+++ b/REVs/REV-17-03-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1301,7 +1301,6 @@
           <t>ML</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
@@ -1347,6 +1346,1237 @@
           <t>TESTE +info IT</t>
         </is>
       </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0TF26852</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA CHUPA CHUPS NARANJA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0TF26855</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA CHUPA CHUPS MANZANA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0TF26854</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA CHUPA CHUPS SANDIA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0TF26856</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA CHUPA CHUPS COLA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0TF26853</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA CHUPA CHUPS FRESA NATA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0TF26850</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA BARBIE NIACINAMIDA &amp; COCO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0TF26851</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MONTAGNE MASCARILLA BARBIE ROSA &amp; VITAMINA E</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0TF26857</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MONTAGNE TUBO PEEL OFF CARBON 50ML</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No Tiene ES - TRADUCIDO</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0TF26858</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MONTAGNE TUBO PEEL OFF ARBOL DE TE 50ML</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No Tiene ES - TRADUCIDO</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0TF26858</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MONTAGNE TUBO PEEL OFF ARBOL DE TE 50ML</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0TF26857</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MONTAGNE TUBO PEEL OFF CARBON 50ML</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0TS04090</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>DIOR SOLAR BODY SELF TANING GEL TUBO 150ML</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0TS04093</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SHISEIDO EXPERT SUN PROTECTOR CLEAN STICK 20G</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0TS04093</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SHISEIDO EXPERT SUN PROTECTOR CLEAN STICK 20G</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0TS04092</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SHISEIDO EXPERT SUN PROTECTOR LOTION SPF30 300ML</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>0TF26826</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CLINIQUE MOISTURE SURGE BODY HYDRATOR 200ML</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0MO26921</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>LANCOME SET MASCARA BIG MOUNSIER</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE OJOS</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0MO26919</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>LANCOME MASCARA HYPNOSE DRAMA SET SPRING25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE OJOS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0MO27030</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>LANCOME SET MASCARA LASH IDOLE 10ML</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE OJOS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0MO26921</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>LANCOME SET MASCARA BIG MOUNSIER</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>MAQUILLAJE OJOS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>6XY00554</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>PLUS ONE PRIVATE PLEASURE VIBE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>JUEGOS EROTICOS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>6XY00556</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PLUS ONE LUXE MENOPAUSE MASSAGER</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>JUEGOS EROTICOS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>6XY00555</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PLUS ONE LUXE RIPPLE MULTI VIBE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>JUEGOS EROTICOS</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>6XS18401</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BLEVIT SF 8 CEREALES Y GALLETA 500GRS + REGALO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>"2x Cereales de 250gr cada uno","1x brinde"</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>4EF05448</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>KENZO FLOWER SET EDP 100ML + 10ML + CREMA C 75ML</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Set &amp; Pack</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>"1x EDP 100ML","1x Leche Corporal 75ML","1x EDP Mini 10ML"</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>4EF05447</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>KENZO FLOWER SET EDP 50ML + BM75ML + MINI 10ML</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>PERF. ESTUCHES MUJER</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>